<commit_message>
fix find uncovered edges
</commit_message>
<xml_diff>
--- a/graph_expr/output/old results/before june 2, 2021/goodcol_outputs- Email_lb20_lb20_cyc_c_q7/Email_lb20_lb20_cyc_c_q7__simgrBYVIEWS_newcols_rmvEmpty.xlsx
+++ b/graph_expr/output/old results/before june 2, 2021/goodcol_outputs- Email_lb20_lb20_cyc_c_q7/Email_lb20_lb20_cyc_c_q7__simgrBYVIEWS_newcols_rmvEmpty.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
   <si>
     <t xml:space="preserve">*****************************************************</t>
   </si>
@@ -209,7 +209,7 @@
     <t xml:space="preserve">all filters</t>
   </si>
   <si>
-    <t xml:space="preserve">partial rewriting, 1 run</t>
+    <t xml:space="preserve">partial rewriting</t>
   </si>
 </sst>
 </file>
@@ -777,7 +777,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K14" activeCellId="0" sqref="K14"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.01171875" defaultRowHeight="17" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1211,9 +1211,7 @@
       <c r="A15" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="B15" s="3"/>
       <c r="C15" s="1" t="n">
         <v>0.18</v>
       </c>

</xml_diff>